<commit_message>
add more Russian weather station of Eastern Siberia
</commit_message>
<xml_diff>
--- a/气象/站点统计.xlsx
+++ b/气象/站点统计.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\文档\GIT SYNC\default\气象\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CAE2499-6F69-43F4-AFE8-236048A93FF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4806D42B-A3C7-4815-9DDD-045C18D46081}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="4" xr2:uid="{8D56AB80-2E26-4029-929F-AED17FA8BDE0}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="5" xr2:uid="{8D56AB80-2E26-4029-929F-AED17FA8BDE0}"/>
   </bookViews>
   <sheets>
     <sheet name="平均气温" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="蒙古极端高温" sheetId="4" r:id="rId3"/>
     <sheet name="单站记录汇总" sheetId="5" r:id="rId4"/>
     <sheet name="蒙古分省均温" sheetId="6" r:id="rId5"/>
+    <sheet name="俄罗斯高纬度" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="262">
   <si>
     <t>漠河</t>
   </si>
@@ -1014,6 +1015,72 @@
     <t>1991-2020蒙古国分省各月平均气温(℃)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>91-20一均</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>91-20十二均</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>61-90一均</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>61-90十二均</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>站号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>地区</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>萨哈共和国</t>
+  </si>
+  <si>
+    <t>俄罗斯</t>
+  </si>
+  <si>
+    <t>DELYANKIR</t>
+  </si>
+  <si>
+    <t>YURTY</t>
+  </si>
+  <si>
+    <t>TOKO</t>
+  </si>
+  <si>
+    <t>奥伊米亚康</t>
+  </si>
+  <si>
+    <t>乌斯季涅拉</t>
+  </si>
+  <si>
+    <t>上扬斯克</t>
+  </si>
+  <si>
+    <t>雅库茨克</t>
+  </si>
+  <si>
+    <t>IEMA</t>
+  </si>
+  <si>
+    <t>61-90二均比十二均高 -42</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>阿加亚坎</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>乌斯季莫马(霍努)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -1023,7 +1090,7 @@
     <numFmt numFmtId="176" formatCode="0.0"/>
     <numFmt numFmtId="177" formatCode="0.0_ "/>
   </numFmts>
-  <fonts count="63" x14ac:knownFonts="1">
+  <fonts count="64" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1568,6 +1635,14 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="25">
     <fill>
@@ -2358,7 +2433,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="207">
+  <cellXfs count="209">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2887,6 +2962,48 @@
     <xf numFmtId="0" fontId="50" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="51" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="36" fillId="2" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="52" fillId="2" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="57" fillId="2" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="59" fillId="2" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="60" fillId="2" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="61" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="62" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2932,27 +3049,6 @@
     <xf numFmtId="0" fontId="48" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="51" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="36" fillId="2" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="52" fillId="2" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="54" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="54" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="56" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2962,23 +3058,8 @@
     <xf numFmtId="0" fontId="56" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="57" fillId="2" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="59" fillId="2" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="60" fillId="2" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="61" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="62" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3435,28 +3516,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="100.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="178" t="s">
+      <c r="A1" s="192" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="178"/>
-      <c r="C1" s="178"/>
-      <c r="D1" s="178"/>
-      <c r="E1" s="178"/>
-      <c r="F1" s="176" t="s">
+      <c r="B1" s="192"/>
+      <c r="C1" s="192"/>
+      <c r="D1" s="192"/>
+      <c r="E1" s="192"/>
+      <c r="F1" s="190" t="s">
         <v>88</v>
       </c>
-      <c r="G1" s="176"/>
-      <c r="H1" s="176"/>
-      <c r="I1" s="176"/>
-      <c r="J1" s="176"/>
-      <c r="K1" s="176"/>
-      <c r="L1" s="176"/>
-      <c r="M1" s="176"/>
-      <c r="N1" s="176"/>
-      <c r="O1" s="176"/>
-      <c r="P1" s="176"/>
-      <c r="Q1" s="176"/>
-      <c r="R1" s="177"/>
+      <c r="G1" s="190"/>
+      <c r="H1" s="190"/>
+      <c r="I1" s="190"/>
+      <c r="J1" s="190"/>
+      <c r="K1" s="190"/>
+      <c r="L1" s="190"/>
+      <c r="M1" s="190"/>
+      <c r="N1" s="190"/>
+      <c r="O1" s="190"/>
+      <c r="P1" s="190"/>
+      <c r="Q1" s="190"/>
+      <c r="R1" s="191"/>
     </row>
     <row r="2" spans="1:19" s="2" customFormat="1" ht="50" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="59" t="s">
@@ -3465,11 +3546,11 @@
       <c r="B2" s="59" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="179" t="s">
+      <c r="C2" s="193" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="180"/>
-      <c r="E2" s="181"/>
+      <c r="D2" s="194"/>
+      <c r="E2" s="195"/>
       <c r="F2" s="58" t="s">
         <v>27</v>
       </c>
@@ -5005,26 +5086,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="82.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="183" t="s">
+      <c r="A1" s="197" t="s">
         <v>129</v>
       </c>
-      <c r="B1" s="184"/>
-      <c r="C1" s="184"/>
-      <c r="D1" s="184"/>
-      <c r="E1" s="184"/>
-      <c r="F1" s="184"/>
-      <c r="G1" s="184"/>
-      <c r="H1" s="184"/>
-      <c r="I1" s="184"/>
-      <c r="J1" s="184"/>
-      <c r="K1" s="184"/>
-      <c r="L1" s="184"/>
-      <c r="M1" s="184"/>
-      <c r="N1" s="184"/>
-      <c r="O1" s="184"/>
-      <c r="P1" s="184"/>
-      <c r="Q1" s="184"/>
-      <c r="R1" s="184"/>
+      <c r="B1" s="198"/>
+      <c r="C1" s="198"/>
+      <c r="D1" s="198"/>
+      <c r="E1" s="198"/>
+      <c r="F1" s="198"/>
+      <c r="G1" s="198"/>
+      <c r="H1" s="198"/>
+      <c r="I1" s="198"/>
+      <c r="J1" s="198"/>
+      <c r="K1" s="198"/>
+      <c r="L1" s="198"/>
+      <c r="M1" s="198"/>
+      <c r="N1" s="198"/>
+      <c r="O1" s="198"/>
+      <c r="P1" s="198"/>
+      <c r="Q1" s="198"/>
+      <c r="R1" s="198"/>
     </row>
     <row r="2" spans="1:19" s="1" customFormat="1" ht="48" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="6" t="s">
@@ -5033,14 +5114,14 @@
       <c r="B2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="182" t="s">
+      <c r="C2" s="196" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="182"/>
+      <c r="D2" s="196"/>
       <c r="E2" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="F2" s="185"/>
+      <c r="F2" s="199"/>
       <c r="G2" s="6" t="s">
         <v>27</v>
       </c>
@@ -5097,7 +5178,7 @@
       <c r="E3" s="11">
         <v>-52.6</v>
       </c>
-      <c r="F3" s="186"/>
+      <c r="F3" s="200"/>
       <c r="G3" s="12">
         <v>-52.6</v>
       </c>
@@ -5154,7 +5235,7 @@
       <c r="E4" s="19">
         <v>-51.3</v>
       </c>
-      <c r="F4" s="186"/>
+      <c r="F4" s="200"/>
       <c r="G4" s="16">
         <v>-51.3</v>
       </c>
@@ -5211,7 +5292,7 @@
       <c r="E5" s="22">
         <v>-53.3</v>
       </c>
-      <c r="F5" s="186"/>
+      <c r="F5" s="200"/>
       <c r="G5" s="23">
         <v>-53.3</v>
       </c>
@@ -5268,7 +5349,7 @@
       <c r="E6" s="24">
         <v>-50.4</v>
       </c>
-      <c r="F6" s="186"/>
+      <c r="F6" s="200"/>
       <c r="G6" s="13">
         <v>-50.4</v>
       </c>
@@ -5325,7 +5406,7 @@
       <c r="E7" s="19">
         <v>-51.3</v>
       </c>
-      <c r="F7" s="186"/>
+      <c r="F7" s="200"/>
       <c r="G7" s="13">
         <v>-50.3</v>
       </c>
@@ -5382,7 +5463,7 @@
       <c r="E8" s="25">
         <v>-50.7</v>
       </c>
-      <c r="F8" s="186"/>
+      <c r="F8" s="200"/>
       <c r="G8" s="15">
         <v>-50.7</v>
       </c>
@@ -5439,7 +5520,7 @@
       <c r="E9" s="24">
         <v>-50.4</v>
       </c>
-      <c r="F9" s="186"/>
+      <c r="F9" s="200"/>
       <c r="G9" s="13">
         <v>-50.4</v>
       </c>
@@ -5496,7 +5577,7 @@
       <c r="E10" s="26">
         <v>-51.9</v>
       </c>
-      <c r="F10" s="186"/>
+      <c r="F10" s="200"/>
       <c r="G10" s="20">
         <v>-51.9</v>
       </c>
@@ -5553,7 +5634,7 @@
       <c r="E11" s="25">
         <v>-50.6</v>
       </c>
-      <c r="F11" s="186"/>
+      <c r="F11" s="200"/>
       <c r="G11" s="15">
         <v>-50.6</v>
       </c>
@@ -5610,7 +5691,7 @@
       <c r="E12" s="28">
         <v>-52.9</v>
       </c>
-      <c r="F12" s="186"/>
+      <c r="F12" s="200"/>
       <c r="G12" s="21">
         <v>-52.9</v>
       </c>
@@ -5667,7 +5748,7 @@
       <c r="E13" s="29">
         <v>-54.7</v>
       </c>
-      <c r="F13" s="186"/>
+      <c r="F13" s="200"/>
       <c r="G13" s="23">
         <v>-53.2</v>
       </c>
@@ -5724,7 +5805,7 @@
       <c r="E14" s="19">
         <v>-51.2</v>
       </c>
-      <c r="F14" s="186"/>
+      <c r="F14" s="200"/>
       <c r="G14" s="16">
         <v>-51.2</v>
       </c>
@@ -5781,7 +5862,7 @@
       <c r="E15" s="30">
         <v>-55.3</v>
       </c>
-      <c r="F15" s="187"/>
+      <c r="F15" s="201"/>
       <c r="G15" s="14">
         <v>-55.3</v>
       </c>
@@ -5863,25 +5944,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="180" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="183" t="s">
+      <c r="A1" s="197" t="s">
         <v>181</v>
       </c>
-      <c r="B1" s="183"/>
-      <c r="C1" s="183"/>
-      <c r="D1" s="183"/>
-      <c r="E1" s="183"/>
-      <c r="F1" s="183"/>
-      <c r="G1" s="183"/>
-      <c r="H1" s="183"/>
-      <c r="I1" s="183"/>
-      <c r="J1" s="183"/>
-      <c r="K1" s="183"/>
-      <c r="L1" s="183"/>
-      <c r="M1" s="183"/>
-      <c r="N1" s="183"/>
-      <c r="O1" s="183"/>
-      <c r="P1" s="183"/>
-      <c r="Q1" s="189"/>
+      <c r="B1" s="197"/>
+      <c r="C1" s="197"/>
+      <c r="D1" s="197"/>
+      <c r="E1" s="197"/>
+      <c r="F1" s="197"/>
+      <c r="G1" s="197"/>
+      <c r="H1" s="197"/>
+      <c r="I1" s="197"/>
+      <c r="J1" s="197"/>
+      <c r="K1" s="197"/>
+      <c r="L1" s="197"/>
+      <c r="M1" s="197"/>
+      <c r="N1" s="197"/>
+      <c r="O1" s="197"/>
+      <c r="P1" s="197"/>
+      <c r="Q1" s="203"/>
     </row>
     <row r="2" spans="1:18" s="1" customFormat="1" ht="100.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="103" t="s">
@@ -5890,10 +5971,10 @@
       <c r="B2" s="103" t="s">
         <v>180</v>
       </c>
-      <c r="C2" s="188" t="s">
+      <c r="C2" s="202" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="188"/>
+      <c r="D2" s="202"/>
       <c r="E2" s="108" t="s">
         <v>167</v>
       </c>
@@ -6834,18 +6915,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="172" customFormat="1" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="190" t="s">
+      <c r="A1" s="204" t="s">
         <v>221</v>
       </c>
-      <c r="B1" s="190"/>
-      <c r="C1" s="190"/>
-      <c r="D1" s="190"/>
-      <c r="E1" s="190"/>
-      <c r="F1" s="190"/>
-      <c r="G1" s="190"/>
-      <c r="H1" s="190"/>
-      <c r="I1" s="190"/>
-      <c r="J1" s="190"/>
+      <c r="B1" s="204"/>
+      <c r="C1" s="204"/>
+      <c r="D1" s="204"/>
+      <c r="E1" s="204"/>
+      <c r="F1" s="204"/>
+      <c r="G1" s="204"/>
+      <c r="H1" s="204"/>
+      <c r="I1" s="204"/>
+      <c r="J1" s="204"/>
     </row>
     <row r="2" spans="1:10" ht="64.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="162" t="s">
@@ -8035,7 +8116,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34899CCC-FF45-4907-A424-75692FA6B55F}">
   <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:O1"/>
     </sheetView>
   </sheetViews>
@@ -8048,1149 +8129,1149 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="198" t="s">
+      <c r="A1" s="205" t="s">
         <v>242</v>
       </c>
-      <c r="B1" s="199"/>
-      <c r="C1" s="199"/>
-      <c r="D1" s="199"/>
-      <c r="E1" s="199"/>
-      <c r="F1" s="199"/>
-      <c r="G1" s="199"/>
-      <c r="H1" s="199"/>
-      <c r="I1" s="199"/>
-      <c r="J1" s="199"/>
-      <c r="K1" s="199"/>
-      <c r="L1" s="199"/>
-      <c r="M1" s="199"/>
-      <c r="N1" s="199"/>
-      <c r="O1" s="200"/>
+      <c r="B1" s="206"/>
+      <c r="C1" s="206"/>
+      <c r="D1" s="206"/>
+      <c r="E1" s="206"/>
+      <c r="F1" s="206"/>
+      <c r="G1" s="206"/>
+      <c r="H1" s="206"/>
+      <c r="I1" s="206"/>
+      <c r="J1" s="206"/>
+      <c r="K1" s="206"/>
+      <c r="L1" s="206"/>
+      <c r="M1" s="206"/>
+      <c r="N1" s="206"/>
+      <c r="O1" s="207"/>
     </row>
     <row r="2" spans="1:15" ht="44" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="194" t="s">
+      <c r="A2" s="179" t="s">
         <v>222</v>
       </c>
-      <c r="B2" s="195" t="s">
+      <c r="B2" s="180" t="s">
         <v>241</v>
       </c>
-      <c r="C2" s="204" t="s">
+      <c r="C2" s="186" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="204" t="s">
+      <c r="D2" s="186" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="204" t="s">
+      <c r="E2" s="186" t="s">
         <v>91</v>
       </c>
-      <c r="F2" s="204" t="s">
+      <c r="F2" s="186" t="s">
         <v>92</v>
       </c>
-      <c r="G2" s="204" t="s">
+      <c r="G2" s="186" t="s">
         <v>93</v>
       </c>
-      <c r="H2" s="204" t="s">
+      <c r="H2" s="186" t="s">
         <v>94</v>
       </c>
-      <c r="I2" s="204" t="s">
+      <c r="I2" s="186" t="s">
         <v>95</v>
       </c>
-      <c r="J2" s="204" t="s">
+      <c r="J2" s="186" t="s">
         <v>96</v>
       </c>
-      <c r="K2" s="204" t="s">
+      <c r="K2" s="186" t="s">
         <v>97</v>
       </c>
-      <c r="L2" s="204" t="s">
+      <c r="L2" s="186" t="s">
         <v>98</v>
       </c>
-      <c r="M2" s="196" t="s">
+      <c r="M2" s="181" t="s">
         <v>99</v>
       </c>
-      <c r="N2" s="196" t="s">
+      <c r="N2" s="181" t="s">
         <v>100</v>
       </c>
-      <c r="O2" s="194" t="s">
+      <c r="O2" s="179" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="197" t="s">
+      <c r="A3" s="182" t="s">
         <v>108</v>
       </c>
-      <c r="B3" s="191">
+      <c r="B3" s="176">
         <v>18</v>
       </c>
-      <c r="C3" s="201">
+      <c r="C3" s="183">
         <v>-27.2</v>
       </c>
-      <c r="D3" s="201">
+      <c r="D3" s="183">
         <v>-23.2</v>
       </c>
-      <c r="E3" s="201">
+      <c r="E3" s="183">
         <v>-12</v>
       </c>
-      <c r="F3" s="192">
+      <c r="F3" s="177">
         <v>2.8</v>
       </c>
-      <c r="G3" s="193">
+      <c r="G3" s="178">
         <v>10.9</v>
       </c>
-      <c r="H3" s="193">
+      <c r="H3" s="178">
         <v>17.3</v>
       </c>
-      <c r="I3" s="193">
+      <c r="I3" s="178">
         <v>19.100000000000001</v>
       </c>
-      <c r="J3" s="193">
+      <c r="J3" s="178">
         <v>16.7</v>
       </c>
-      <c r="K3" s="193">
+      <c r="K3" s="178">
         <v>9.8000000000000007</v>
       </c>
-      <c r="L3" s="192">
+      <c r="L3" s="177">
         <v>1.1000000000000001</v>
       </c>
-      <c r="M3" s="192">
+      <c r="M3" s="177">
         <v>-10</v>
       </c>
-      <c r="N3" s="192">
+      <c r="N3" s="177">
         <v>-21.7</v>
       </c>
-      <c r="O3" s="192">
+      <c r="O3" s="177">
         <v>-1.4</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="197" t="s">
+      <c r="A4" s="182" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="191">
+      <c r="B4" s="176">
         <v>23</v>
       </c>
-      <c r="C4" s="192">
+      <c r="C4" s="177">
         <v>-26.4</v>
       </c>
-      <c r="D4" s="192">
+      <c r="D4" s="177">
         <v>-22.4</v>
       </c>
-      <c r="E4" s="192">
+      <c r="E4" s="177">
         <v>-11.6</v>
       </c>
-      <c r="F4" s="201">
+      <c r="F4" s="183">
         <v>1.3</v>
       </c>
-      <c r="G4" s="192">
+      <c r="G4" s="177">
         <v>8.4</v>
       </c>
-      <c r="H4" s="192">
+      <c r="H4" s="177">
         <v>14.8</v>
       </c>
-      <c r="I4" s="192">
+      <c r="I4" s="177">
         <v>16.8</v>
       </c>
-      <c r="J4" s="192">
+      <c r="J4" s="177">
         <v>14.2</v>
       </c>
-      <c r="K4" s="192">
+      <c r="K4" s="177">
         <v>7.4</v>
       </c>
-      <c r="L4" s="201">
+      <c r="L4" s="183">
         <v>-1.5</v>
       </c>
-      <c r="M4" s="201">
+      <c r="M4" s="183">
         <v>-12.9</v>
       </c>
-      <c r="N4" s="201">
+      <c r="N4" s="183">
         <v>-22.8</v>
       </c>
-      <c r="O4" s="201">
+      <c r="O4" s="183">
         <v>-2.9</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="197" t="s">
+      <c r="A5" s="182" t="s">
         <v>102</v>
       </c>
-      <c r="B5" s="191">
+      <c r="B5" s="176">
         <v>13</v>
       </c>
-      <c r="C5" s="192">
+      <c r="C5" s="177">
         <v>-24.5</v>
       </c>
-      <c r="D5" s="192">
+      <c r="D5" s="177">
         <v>-19.100000000000001</v>
       </c>
-      <c r="E5" s="192">
+      <c r="E5" s="177">
         <v>-6.9</v>
       </c>
-      <c r="F5" s="192">
+      <c r="F5" s="177">
         <v>4.3</v>
       </c>
-      <c r="G5" s="193">
+      <c r="G5" s="178">
         <v>11.4</v>
       </c>
-      <c r="H5" s="193">
+      <c r="H5" s="178">
         <v>17.899999999999999</v>
       </c>
-      <c r="I5" s="193">
+      <c r="I5" s="178">
         <v>20.2</v>
       </c>
-      <c r="J5" s="193">
+      <c r="J5" s="178">
         <v>17.399999999999999</v>
       </c>
-      <c r="K5" s="193">
+      <c r="K5" s="178">
         <v>10.199999999999999</v>
       </c>
-      <c r="L5" s="192">
+      <c r="L5" s="177">
         <v>0.9</v>
       </c>
-      <c r="M5" s="192">
+      <c r="M5" s="177">
         <v>-11</v>
       </c>
-      <c r="N5" s="192">
+      <c r="N5" s="177">
         <v>-21.1</v>
       </c>
-      <c r="O5" s="192">
+      <c r="O5" s="177">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="197" t="s">
+      <c r="A6" s="182" t="s">
         <v>229</v>
       </c>
-      <c r="B6" s="191">
+      <c r="B6" s="176">
         <v>4</v>
       </c>
-      <c r="C6" s="192">
+      <c r="C6" s="177">
         <v>-24.4</v>
       </c>
-      <c r="D6" s="192">
+      <c r="D6" s="177">
         <v>-19</v>
       </c>
-      <c r="E6" s="192">
+      <c r="E6" s="177">
         <v>-6.4</v>
       </c>
-      <c r="F6" s="192">
+      <c r="F6" s="177">
         <v>4.7</v>
       </c>
-      <c r="G6" s="193">
+      <c r="G6" s="178">
         <v>11.9</v>
       </c>
-      <c r="H6" s="193">
+      <c r="H6" s="178">
         <v>18.2</v>
       </c>
-      <c r="I6" s="193">
+      <c r="I6" s="178">
         <v>20.5</v>
       </c>
-      <c r="J6" s="193">
+      <c r="J6" s="178">
         <v>17.7</v>
       </c>
-      <c r="K6" s="193">
+      <c r="K6" s="178">
         <v>10.5</v>
       </c>
-      <c r="L6" s="192">
+      <c r="L6" s="177">
         <v>1.2</v>
       </c>
-      <c r="M6" s="192">
+      <c r="M6" s="177">
         <v>-10.8</v>
       </c>
-      <c r="N6" s="192">
+      <c r="N6" s="177">
         <v>-21.1</v>
       </c>
-      <c r="O6" s="192">
+      <c r="O6" s="177">
         <v>0.3</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="197" t="s">
+      <c r="A7" s="182" t="s">
         <v>104</v>
       </c>
-      <c r="B7" s="191">
+      <c r="B7" s="176">
         <v>24</v>
       </c>
-      <c r="C7" s="192">
+      <c r="C7" s="177">
         <v>-24.2</v>
       </c>
-      <c r="D7" s="192">
+      <c r="D7" s="177">
         <v>-19</v>
       </c>
-      <c r="E7" s="192">
+      <c r="E7" s="177">
         <v>-9</v>
       </c>
-      <c r="F7" s="192">
+      <c r="F7" s="177">
         <v>1.6</v>
       </c>
-      <c r="G7" s="201">
+      <c r="G7" s="183">
         <v>8.1999999999999993</v>
       </c>
-      <c r="H7" s="201">
+      <c r="H7" s="183">
         <v>14.1</v>
       </c>
-      <c r="I7" s="201">
+      <c r="I7" s="183">
         <v>16.100000000000001</v>
       </c>
-      <c r="J7" s="201">
+      <c r="J7" s="183">
         <v>13.7</v>
       </c>
-      <c r="K7" s="201">
+      <c r="K7" s="183">
         <v>7.1</v>
       </c>
-      <c r="L7" s="192">
+      <c r="L7" s="177">
         <v>-1.3</v>
       </c>
-      <c r="M7" s="192">
+      <c r="M7" s="177">
         <v>-11.9</v>
       </c>
-      <c r="N7" s="192">
+      <c r="N7" s="177">
         <v>-20.6</v>
       </c>
-      <c r="O7" s="192">
+      <c r="O7" s="177">
         <v>-2.1</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="197" t="s">
+      <c r="A8" s="182" t="s">
         <v>137</v>
       </c>
-      <c r="B8" s="191">
+      <c r="B8" s="176">
         <v>6</v>
       </c>
-      <c r="C8" s="192">
+      <c r="C8" s="177">
         <v>-23.1</v>
       </c>
-      <c r="D8" s="192">
+      <c r="D8" s="177">
         <v>-18.3</v>
       </c>
-      <c r="E8" s="192">
+      <c r="E8" s="177">
         <v>-8.3000000000000007</v>
       </c>
-      <c r="F8" s="192">
+      <c r="F8" s="177">
         <v>2.1</v>
       </c>
-      <c r="G8" s="193">
+      <c r="G8" s="178">
         <v>9.3000000000000007</v>
       </c>
-      <c r="H8" s="193">
+      <c r="H8" s="178">
         <v>15.5</v>
       </c>
-      <c r="I8" s="193">
+      <c r="I8" s="178">
         <v>17.899999999999999</v>
       </c>
-      <c r="J8" s="193">
+      <c r="J8" s="178">
         <v>15.4</v>
       </c>
-      <c r="K8" s="193">
+      <c r="K8" s="178">
         <v>8.6999999999999993</v>
       </c>
-      <c r="L8" s="192">
+      <c r="L8" s="177">
         <v>-0.4</v>
       </c>
-      <c r="M8" s="192">
+      <c r="M8" s="177">
         <v>-12.1</v>
       </c>
-      <c r="N8" s="192">
+      <c r="N8" s="177">
         <v>-20.8</v>
       </c>
-      <c r="O8" s="192">
+      <c r="O8" s="177">
         <v>-1.2</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="197" t="s">
+      <c r="A9" s="182" t="s">
         <v>237</v>
       </c>
-      <c r="B9" s="191">
+      <c r="B9" s="176">
         <v>21</v>
       </c>
-      <c r="C9" s="192">
+      <c r="C9" s="177">
         <v>-22.3</v>
       </c>
-      <c r="D9" s="192">
+      <c r="D9" s="177">
         <v>-17.2</v>
       </c>
-      <c r="E9" s="192">
+      <c r="E9" s="177">
         <v>-7</v>
       </c>
-      <c r="F9" s="192">
+      <c r="F9" s="177">
         <v>3</v>
       </c>
-      <c r="G9" s="193">
+      <c r="G9" s="178">
         <v>10.199999999999999</v>
       </c>
-      <c r="H9" s="193">
+      <c r="H9" s="178">
         <v>16.899999999999999</v>
       </c>
-      <c r="I9" s="193">
+      <c r="I9" s="178">
         <v>19.2</v>
       </c>
-      <c r="J9" s="193">
+      <c r="J9" s="178">
         <v>16.8</v>
       </c>
-      <c r="K9" s="193">
+      <c r="K9" s="178">
         <v>10</v>
       </c>
-      <c r="L9" s="192">
+      <c r="L9" s="177">
         <v>0.2</v>
       </c>
-      <c r="M9" s="192">
+      <c r="M9" s="177">
         <v>-10.9</v>
       </c>
-      <c r="N9" s="192">
+      <c r="N9" s="177">
         <v>-20</v>
       </c>
-      <c r="O9" s="192">
+      <c r="O9" s="177">
         <v>-0.1</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="197" t="s">
+      <c r="A10" s="182" t="s">
         <v>239</v>
       </c>
-      <c r="B10" s="191">
+      <c r="B10" s="176">
         <v>18</v>
       </c>
-      <c r="C10" s="192">
+      <c r="C10" s="177">
         <v>-21.4</v>
       </c>
-      <c r="D10" s="192">
+      <c r="D10" s="177">
         <v>-16.7</v>
       </c>
-      <c r="E10" s="192">
+      <c r="E10" s="177">
         <v>-7.4</v>
       </c>
-      <c r="F10" s="192">
+      <c r="F10" s="177">
         <v>2.9</v>
       </c>
-      <c r="G10" s="193">
+      <c r="G10" s="178">
         <v>10.8</v>
       </c>
-      <c r="H10" s="193">
+      <c r="H10" s="178">
         <v>17.100000000000001</v>
       </c>
-      <c r="I10" s="193">
+      <c r="I10" s="178">
         <v>19.399999999999999</v>
       </c>
-      <c r="J10" s="193">
+      <c r="J10" s="178">
         <v>17</v>
       </c>
-      <c r="K10" s="193">
+      <c r="K10" s="178">
         <v>10.3</v>
       </c>
-      <c r="L10" s="192">
+      <c r="L10" s="177">
         <v>0.6</v>
       </c>
-      <c r="M10" s="192">
+      <c r="M10" s="177">
         <v>-10.9</v>
       </c>
-      <c r="N10" s="192">
+      <c r="N10" s="177">
         <v>-19.399999999999999</v>
       </c>
-      <c r="O10" s="192">
+      <c r="O10" s="177">
         <v>0.2</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="197" t="s">
+      <c r="A11" s="182" t="s">
         <v>224</v>
       </c>
-      <c r="B11" s="191">
+      <c r="B11" s="176">
         <v>12</v>
       </c>
-      <c r="C11" s="192">
+      <c r="C11" s="177">
         <v>-21.4</v>
       </c>
-      <c r="D11" s="192">
+      <c r="D11" s="177">
         <v>-16.3</v>
       </c>
-      <c r="E11" s="192">
+      <c r="E11" s="177">
         <v>-7.1</v>
       </c>
-      <c r="F11" s="192">
+      <c r="F11" s="177">
         <v>2.2000000000000002</v>
       </c>
-      <c r="G11" s="192">
+      <c r="G11" s="177">
         <v>8.4</v>
       </c>
-      <c r="H11" s="192">
+      <c r="H11" s="177">
         <v>14.4</v>
       </c>
-      <c r="I11" s="201">
+      <c r="I11" s="183">
         <v>16.100000000000001</v>
       </c>
-      <c r="J11" s="192">
+      <c r="J11" s="177">
         <v>14.2</v>
       </c>
-      <c r="K11" s="192">
+      <c r="K11" s="177">
         <v>7.8</v>
       </c>
-      <c r="L11" s="192">
+      <c r="L11" s="177">
         <v>-0.2</v>
       </c>
-      <c r="M11" s="192">
+      <c r="M11" s="177">
         <v>-10.1</v>
       </c>
-      <c r="N11" s="192">
+      <c r="N11" s="177">
         <v>-18.3</v>
       </c>
-      <c r="O11" s="192">
+      <c r="O11" s="177">
         <v>-0.9</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="205" t="s">
+      <c r="A12" s="187" t="s">
         <v>240</v>
       </c>
-      <c r="B12" s="206">
+      <c r="B12" s="188">
         <v>317</v>
       </c>
-      <c r="C12" s="202">
+      <c r="C12" s="184">
         <v>-21.3</v>
       </c>
-      <c r="D12" s="202">
+      <c r="D12" s="184">
         <v>-16.7</v>
       </c>
-      <c r="E12" s="202">
+      <c r="E12" s="184">
         <v>-6.9</v>
       </c>
-      <c r="F12" s="202">
+      <c r="F12" s="184">
         <v>3.6</v>
       </c>
-      <c r="G12" s="202">
+      <c r="G12" s="184">
         <v>10.7</v>
       </c>
-      <c r="H12" s="202">
+      <c r="H12" s="184">
         <v>16.899999999999999</v>
       </c>
-      <c r="I12" s="202">
+      <c r="I12" s="184">
         <v>19.100000000000001</v>
       </c>
-      <c r="J12" s="202">
+      <c r="J12" s="184">
         <v>16.8</v>
       </c>
-      <c r="K12" s="202">
+      <c r="K12" s="184">
         <v>10.1</v>
       </c>
-      <c r="L12" s="202">
+      <c r="L12" s="184">
         <v>1.1000000000000001</v>
       </c>
-      <c r="M12" s="202">
+      <c r="M12" s="184">
         <v>-9.6</v>
       </c>
-      <c r="N12" s="202">
+      <c r="N12" s="184">
         <v>-18.399999999999999</v>
       </c>
-      <c r="O12" s="202">
+      <c r="O12" s="184">
         <v>0.5</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="197" t="s">
+      <c r="A13" s="182" t="s">
         <v>226</v>
       </c>
-      <c r="B13" s="191">
+      <c r="B13" s="176">
         <v>16</v>
       </c>
-      <c r="C13" s="192">
+      <c r="C13" s="177">
         <v>-21.2</v>
       </c>
-      <c r="D13" s="192">
+      <c r="D13" s="177">
         <v>-16.3</v>
       </c>
-      <c r="E13" s="192">
+      <c r="E13" s="177">
         <v>-6.2</v>
       </c>
-      <c r="F13" s="192">
+      <c r="F13" s="177">
         <v>4</v>
       </c>
-      <c r="G13" s="193">
+      <c r="G13" s="178">
         <v>10.9</v>
       </c>
-      <c r="H13" s="193">
+      <c r="H13" s="178">
         <v>16.8</v>
       </c>
-      <c r="I13" s="193">
+      <c r="I13" s="178">
         <v>18.8</v>
       </c>
-      <c r="J13" s="193">
+      <c r="J13" s="178">
         <v>16.3</v>
       </c>
-      <c r="K13" s="193">
+      <c r="K13" s="178">
         <v>9.6</v>
       </c>
-      <c r="L13" s="192">
+      <c r="L13" s="177">
         <v>0.6</v>
       </c>
-      <c r="M13" s="192">
+      <c r="M13" s="177">
         <v>-10</v>
       </c>
-      <c r="N13" s="192">
+      <c r="N13" s="177">
         <v>-18.100000000000001</v>
       </c>
-      <c r="O13" s="192">
+      <c r="O13" s="177">
         <v>0.4</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="197" t="s">
+      <c r="A14" s="182" t="s">
         <v>238</v>
       </c>
-      <c r="B14" s="191">
+      <c r="B14" s="176">
         <v>16</v>
       </c>
-      <c r="C14" s="192">
+      <c r="C14" s="177">
         <v>-21.2</v>
       </c>
-      <c r="D14" s="192">
+      <c r="D14" s="177">
         <v>-16.3</v>
       </c>
-      <c r="E14" s="192">
+      <c r="E14" s="177">
         <v>-5.0999999999999996</v>
       </c>
-      <c r="F14" s="193">
+      <c r="F14" s="178">
         <v>5.4</v>
       </c>
-      <c r="G14" s="193">
+      <c r="G14" s="178">
         <v>11.9</v>
       </c>
-      <c r="H14" s="193">
+      <c r="H14" s="178">
         <v>17.899999999999999</v>
       </c>
-      <c r="I14" s="193">
+      <c r="I14" s="178">
         <v>19.7</v>
       </c>
-      <c r="J14" s="193">
+      <c r="J14" s="178">
         <v>17.5</v>
       </c>
-      <c r="K14" s="193">
+      <c r="K14" s="178">
         <v>11.2</v>
       </c>
-      <c r="L14" s="192">
+      <c r="L14" s="177">
         <v>2.8</v>
       </c>
-      <c r="M14" s="192">
+      <c r="M14" s="177">
         <v>-7.7</v>
       </c>
-      <c r="N14" s="192">
+      <c r="N14" s="177">
         <v>-17.399999999999999</v>
       </c>
-      <c r="O14" s="192">
+      <c r="O14" s="177">
         <v>1.6</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="197" t="s">
+      <c r="A15" s="182" t="s">
         <v>231</v>
       </c>
-      <c r="B15" s="191">
+      <c r="B15" s="176">
         <v>15</v>
       </c>
-      <c r="C15" s="192">
+      <c r="C15" s="177">
         <v>-20.9</v>
       </c>
-      <c r="D15" s="192">
+      <c r="D15" s="177">
         <v>-16.600000000000001</v>
       </c>
-      <c r="E15" s="192">
+      <c r="E15" s="177">
         <v>-7.2</v>
       </c>
-      <c r="F15" s="192">
+      <c r="F15" s="177">
         <v>3.7</v>
       </c>
-      <c r="G15" s="193">
+      <c r="G15" s="178">
         <v>11.9</v>
       </c>
-      <c r="H15" s="193">
+      <c r="H15" s="178">
         <v>18.600000000000001</v>
       </c>
-      <c r="I15" s="193">
+      <c r="I15" s="178">
         <v>21.1</v>
       </c>
-      <c r="J15" s="193">
+      <c r="J15" s="178">
         <v>18.600000000000001</v>
       </c>
-      <c r="K15" s="193">
+      <c r="K15" s="178">
         <v>11.7</v>
       </c>
-      <c r="L15" s="192">
+      <c r="L15" s="177">
         <v>1.7</v>
       </c>
-      <c r="M15" s="192">
+      <c r="M15" s="177">
         <v>-10</v>
       </c>
-      <c r="N15" s="192">
+      <c r="N15" s="177">
         <v>-18.8</v>
       </c>
-      <c r="O15" s="192">
+      <c r="O15" s="177">
         <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="197" t="s">
+      <c r="A16" s="182" t="s">
         <v>236</v>
       </c>
-      <c r="B16" s="191">
+      <c r="B16" s="176">
         <v>13</v>
       </c>
-      <c r="C16" s="192">
+      <c r="C16" s="177">
         <v>-20.6</v>
       </c>
-      <c r="D16" s="192">
+      <c r="D16" s="177">
         <v>-16</v>
       </c>
-      <c r="E16" s="192">
+      <c r="E16" s="177">
         <v>-6.4</v>
       </c>
-      <c r="F16" s="192">
+      <c r="F16" s="177">
         <v>4.0999999999999996</v>
       </c>
-      <c r="G16" s="193">
+      <c r="G16" s="178">
         <v>12</v>
       </c>
-      <c r="H16" s="193">
+      <c r="H16" s="178">
         <v>18.3</v>
       </c>
-      <c r="I16" s="193">
+      <c r="I16" s="178">
         <v>21.1</v>
       </c>
-      <c r="J16" s="193">
+      <c r="J16" s="178">
         <v>19</v>
       </c>
-      <c r="K16" s="193">
+      <c r="K16" s="178">
         <v>12.3</v>
       </c>
-      <c r="L16" s="192">
+      <c r="L16" s="177">
         <v>2.5</v>
       </c>
-      <c r="M16" s="192">
+      <c r="M16" s="177">
         <v>-9.1999999999999993</v>
       </c>
-      <c r="N16" s="192">
+      <c r="N16" s="177">
         <v>-18.2</v>
       </c>
-      <c r="O16" s="192">
+      <c r="O16" s="177">
         <v>1.6</v>
       </c>
     </row>
     <row r="17" spans="1:15" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="197" t="s">
+      <c r="A17" s="182" t="s">
         <v>223</v>
       </c>
-      <c r="B17" s="191">
+      <c r="B17" s="176">
         <v>17</v>
       </c>
-      <c r="C17" s="192">
+      <c r="C17" s="177">
         <v>-20.399999999999999</v>
       </c>
-      <c r="D17" s="192">
+      <c r="D17" s="177">
         <v>-16.100000000000001</v>
       </c>
-      <c r="E17" s="192">
+      <c r="E17" s="177">
         <v>-7.3</v>
       </c>
-      <c r="F17" s="192">
+      <c r="F17" s="177">
         <v>2.2000000000000002</v>
       </c>
-      <c r="G17" s="192">
+      <c r="G17" s="177">
         <v>8.8000000000000007</v>
       </c>
-      <c r="H17" s="192">
+      <c r="H17" s="177">
         <v>14.4</v>
       </c>
-      <c r="I17" s="192">
+      <c r="I17" s="177">
         <v>16.3</v>
       </c>
-      <c r="J17" s="192">
+      <c r="J17" s="177">
         <v>14</v>
       </c>
-      <c r="K17" s="192">
+      <c r="K17" s="177">
         <v>7.8</v>
       </c>
-      <c r="L17" s="192">
+      <c r="L17" s="177">
         <v>-0.6</v>
       </c>
-      <c r="M17" s="192">
+      <c r="M17" s="177">
         <v>-10</v>
       </c>
-      <c r="N17" s="192">
+      <c r="N17" s="177">
         <v>-17.5</v>
       </c>
-      <c r="O17" s="192">
+      <c r="O17" s="177">
         <v>-0.7</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="197" t="s">
+      <c r="A18" s="182" t="s">
         <v>228</v>
       </c>
-      <c r="B18" s="191">
+      <c r="B18" s="176">
         <v>1</v>
       </c>
-      <c r="C18" s="192">
+      <c r="C18" s="177">
         <v>-19.899999999999999</v>
       </c>
-      <c r="D18" s="192">
+      <c r="D18" s="177">
         <v>-15</v>
       </c>
-      <c r="E18" s="192">
+      <c r="E18" s="177">
         <v>-5.5</v>
       </c>
-      <c r="F18" s="192">
+      <c r="F18" s="177">
         <v>4.2</v>
       </c>
-      <c r="G18" s="193">
+      <c r="G18" s="178">
         <v>11.9</v>
       </c>
-      <c r="H18" s="193">
+      <c r="H18" s="178">
         <v>18.100000000000001</v>
       </c>
-      <c r="I18" s="193">
+      <c r="I18" s="178">
         <v>20.7</v>
       </c>
-      <c r="J18" s="193">
+      <c r="J18" s="178">
         <v>18.399999999999999</v>
       </c>
-      <c r="K18" s="193">
+      <c r="K18" s="178">
         <v>11.9</v>
       </c>
-      <c r="L18" s="192">
+      <c r="L18" s="177">
         <v>2.2000000000000002</v>
       </c>
-      <c r="M18" s="192">
+      <c r="M18" s="177">
         <v>-9.3000000000000007</v>
       </c>
-      <c r="N18" s="192">
+      <c r="N18" s="177">
         <v>-17.899999999999999</v>
       </c>
-      <c r="O18" s="192">
+      <c r="O18" s="177">
         <v>1.6</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="197" t="s">
+      <c r="A19" s="182" t="s">
         <v>227</v>
       </c>
-      <c r="B19" s="191">
+      <c r="B19" s="176">
         <v>20</v>
       </c>
-      <c r="C19" s="192">
+      <c r="C19" s="177">
         <v>-19.5</v>
       </c>
-      <c r="D19" s="192">
+      <c r="D19" s="177">
         <v>-15.1</v>
       </c>
-      <c r="E19" s="192">
+      <c r="E19" s="177">
         <v>-5.7</v>
       </c>
-      <c r="F19" s="192">
+      <c r="F19" s="177">
         <v>4.4000000000000004</v>
       </c>
-      <c r="G19" s="193">
+      <c r="G19" s="178">
         <v>11</v>
       </c>
-      <c r="H19" s="193">
+      <c r="H19" s="178">
         <v>17.3</v>
       </c>
-      <c r="I19" s="193">
+      <c r="I19" s="178">
         <v>19.399999999999999</v>
       </c>
-      <c r="J19" s="193">
+      <c r="J19" s="178">
         <v>17.2</v>
       </c>
-      <c r="K19" s="193">
+      <c r="K19" s="178">
         <v>10.3</v>
       </c>
-      <c r="L19" s="192">
+      <c r="L19" s="177">
         <v>1.7</v>
       </c>
-      <c r="M19" s="192">
+      <c r="M19" s="177">
         <v>-8.1999999999999993</v>
       </c>
-      <c r="N19" s="192">
+      <c r="N19" s="177">
         <v>-16.5</v>
       </c>
-      <c r="O19" s="192">
+      <c r="O19" s="177">
         <v>1.4</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="197" t="s">
+      <c r="A20" s="182" t="s">
         <v>225</v>
       </c>
-      <c r="B20" s="191">
+      <c r="B20" s="176">
         <v>19</v>
       </c>
-      <c r="C20" s="192">
+      <c r="C20" s="177">
         <v>-19.2</v>
       </c>
-      <c r="D20" s="192">
+      <c r="D20" s="177">
         <v>-15.1</v>
       </c>
-      <c r="E20" s="192">
+      <c r="E20" s="177">
         <v>-6.4</v>
       </c>
-      <c r="F20" s="192">
+      <c r="F20" s="177">
         <v>3.5</v>
       </c>
-      <c r="G20" s="193">
+      <c r="G20" s="178">
         <v>10.4</v>
       </c>
-      <c r="H20" s="193">
+      <c r="H20" s="178">
         <v>16.5</v>
       </c>
-      <c r="I20" s="193">
+      <c r="I20" s="178">
         <v>18.7</v>
       </c>
-      <c r="J20" s="193">
+      <c r="J20" s="178">
         <v>16.600000000000001</v>
       </c>
-      <c r="K20" s="193">
+      <c r="K20" s="178">
         <v>9.8000000000000007</v>
       </c>
-      <c r="L20" s="192">
+      <c r="L20" s="177">
         <v>0.7</v>
       </c>
-      <c r="M20" s="192">
+      <c r="M20" s="177">
         <v>-9.1999999999999993</v>
       </c>
-      <c r="N20" s="192">
+      <c r="N20" s="177">
         <v>-16.7</v>
       </c>
-      <c r="O20" s="192">
+      <c r="O20" s="177">
         <v>0.8</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="197" t="s">
+      <c r="A21" s="182" t="s">
         <v>233</v>
       </c>
-      <c r="B21" s="191">
+      <c r="B21" s="176">
         <v>2</v>
       </c>
-      <c r="C21" s="192">
+      <c r="C21" s="177">
         <v>-18.600000000000001</v>
       </c>
-      <c r="D21" s="192">
+      <c r="D21" s="177">
         <v>-14.9</v>
       </c>
-      <c r="E21" s="192">
+      <c r="E21" s="177">
         <v>-6.3</v>
       </c>
-      <c r="F21" s="192">
+      <c r="F21" s="177">
         <v>3.7</v>
       </c>
-      <c r="G21" s="193">
+      <c r="G21" s="178">
         <v>10.6</v>
       </c>
-      <c r="H21" s="193">
+      <c r="H21" s="178">
         <v>16.5</v>
       </c>
-      <c r="I21" s="193">
+      <c r="I21" s="178">
         <v>18.3</v>
       </c>
-      <c r="J21" s="193">
+      <c r="J21" s="178">
         <v>15.8</v>
       </c>
-      <c r="K21" s="193">
+      <c r="K21" s="178">
         <v>9.4</v>
       </c>
-      <c r="L21" s="192">
+      <c r="L21" s="177">
         <v>0.9</v>
       </c>
-      <c r="M21" s="192">
+      <c r="M21" s="177">
         <v>-9.1999999999999993</v>
       </c>
-      <c r="N21" s="192">
+      <c r="N21" s="177">
         <v>-16.2</v>
       </c>
-      <c r="O21" s="192">
+      <c r="O21" s="177">
         <v>0.8</v>
       </c>
     </row>
     <row r="22" spans="1:15" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="197" t="s">
+      <c r="A22" s="182" t="s">
         <v>234</v>
       </c>
-      <c r="B22" s="191">
+      <c r="B22" s="176">
         <v>18</v>
       </c>
-      <c r="C22" s="192">
+      <c r="C22" s="177">
         <v>-17.7</v>
       </c>
-      <c r="D22" s="192">
+      <c r="D22" s="177">
         <v>-14</v>
       </c>
-      <c r="E22" s="192">
+      <c r="E22" s="177">
         <v>-5.5</v>
       </c>
-      <c r="F22" s="192">
+      <c r="F22" s="177">
         <v>3.8</v>
       </c>
-      <c r="G22" s="193">
+      <c r="G22" s="178">
         <v>10.5</v>
       </c>
-      <c r="H22" s="193">
+      <c r="H22" s="178">
         <v>16.3</v>
       </c>
-      <c r="I22" s="193">
+      <c r="I22" s="178">
         <v>18.600000000000001</v>
       </c>
-      <c r="J22" s="193">
+      <c r="J22" s="178">
         <v>16.600000000000001</v>
       </c>
-      <c r="K22" s="193">
+      <c r="K22" s="178">
         <v>10.3</v>
       </c>
-      <c r="L22" s="192">
+      <c r="L22" s="177">
         <v>1.6</v>
       </c>
-      <c r="M22" s="192">
+      <c r="M22" s="177">
         <v>-8.1</v>
       </c>
-      <c r="N22" s="192">
+      <c r="N22" s="177">
         <v>-15.4</v>
       </c>
-      <c r="O22" s="192">
+      <c r="O22" s="177">
         <v>1.4</v>
       </c>
     </row>
     <row r="23" spans="1:15" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="197" t="s">
+      <c r="A23" s="182" t="s">
         <v>232</v>
       </c>
-      <c r="B23" s="191">
+      <c r="B23" s="176">
         <v>14</v>
       </c>
-      <c r="C23" s="192">
+      <c r="C23" s="177">
         <v>-17.7</v>
       </c>
-      <c r="D23" s="192">
+      <c r="D23" s="177">
         <v>-13.2</v>
       </c>
-      <c r="E23" s="193">
+      <c r="E23" s="178">
         <v>-4</v>
       </c>
-      <c r="F23" s="193">
+      <c r="F23" s="178">
         <v>5.3</v>
       </c>
-      <c r="G23" s="193">
+      <c r="G23" s="178">
         <v>12.6</v>
       </c>
-      <c r="H23" s="193">
+      <c r="H23" s="178">
         <v>19</v>
       </c>
-      <c r="I23" s="193">
+      <c r="I23" s="178">
         <v>21.4</v>
       </c>
-      <c r="J23" s="193">
+      <c r="J23" s="178">
         <v>18.8</v>
       </c>
-      <c r="K23" s="193">
+      <c r="K23" s="178">
         <v>12.6</v>
       </c>
-      <c r="L23" s="193">
+      <c r="L23" s="178">
         <v>3</v>
       </c>
-      <c r="M23" s="192">
+      <c r="M23" s="177">
         <v>-7.6</v>
       </c>
-      <c r="N23" s="192">
+      <c r="N23" s="177">
         <v>-15.6</v>
       </c>
-      <c r="O23" s="193">
+      <c r="O23" s="178">
         <v>2.9</v>
       </c>
     </row>
     <row r="24" spans="1:15" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="197" t="s">
+      <c r="A24" s="182" t="s">
         <v>230</v>
       </c>
-      <c r="B24" s="191">
+      <c r="B24" s="176">
         <v>13</v>
       </c>
-      <c r="C24" s="192">
+      <c r="C24" s="177">
         <v>-17</v>
       </c>
-      <c r="D24" s="192">
+      <c r="D24" s="177">
         <v>-12</v>
       </c>
-      <c r="E24" s="193">
+      <c r="E24" s="178">
         <v>-2.9</v>
       </c>
-      <c r="F24" s="193">
+      <c r="F24" s="178">
         <v>6.9</v>
       </c>
-      <c r="G24" s="203">
+      <c r="G24" s="185">
         <v>14.7</v>
       </c>
-      <c r="H24" s="203">
+      <c r="H24" s="185">
         <v>21</v>
       </c>
-      <c r="I24" s="203">
+      <c r="I24" s="185">
         <v>23.7</v>
       </c>
-      <c r="J24" s="203">
+      <c r="J24" s="185">
         <v>21.5</v>
       </c>
-      <c r="K24" s="203">
+      <c r="K24" s="185">
         <v>14.5</v>
       </c>
-      <c r="L24" s="193">
+      <c r="L24" s="178">
         <v>4.8</v>
       </c>
-      <c r="M24" s="193">
+      <c r="M24" s="178">
         <v>-6.3</v>
       </c>
-      <c r="N24" s="192">
+      <c r="N24" s="177">
         <v>-14.9</v>
       </c>
-      <c r="O24" s="193">
+      <c r="O24" s="178">
         <v>4.5</v>
       </c>
     </row>
     <row r="25" spans="1:15" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="197" t="s">
+      <c r="A25" s="182" t="s">
         <v>235</v>
       </c>
-      <c r="B25" s="191">
+      <c r="B25" s="176">
         <v>14</v>
       </c>
-      <c r="C25" s="203">
+      <c r="C25" s="185">
         <v>-14.2</v>
       </c>
-      <c r="D25" s="203">
+      <c r="D25" s="185">
         <v>-9.6999999999999993</v>
       </c>
-      <c r="E25" s="203">
+      <c r="E25" s="185">
         <v>-1.7</v>
       </c>
-      <c r="F25" s="203">
+      <c r="F25" s="185">
         <v>7.6</v>
       </c>
-      <c r="G25" s="193">
+      <c r="G25" s="178">
         <v>14.5</v>
       </c>
-      <c r="H25" s="193">
+      <c r="H25" s="178">
         <v>20.7</v>
       </c>
-      <c r="I25" s="193">
+      <c r="I25" s="178">
         <v>23.2</v>
       </c>
-      <c r="J25" s="193">
+      <c r="J25" s="178">
         <v>20.9</v>
       </c>
-      <c r="K25" s="193">
+      <c r="K25" s="178">
         <v>14.4</v>
       </c>
-      <c r="L25" s="203">
+      <c r="L25" s="185">
         <v>5.3</v>
       </c>
-      <c r="M25" s="203">
+      <c r="M25" s="185">
         <v>-4.5</v>
       </c>
-      <c r="N25" s="203">
+      <c r="N25" s="185">
         <v>-12.1</v>
       </c>
-      <c r="O25" s="203">
+      <c r="O25" s="185">
         <v>5.4</v>
       </c>
     </row>
@@ -9362,4 +9443,318 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B75E2AF-B562-477E-B49D-E78846CED977}">
+  <dimension ref="A1:I23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="2" max="2" width="12.59765625" customWidth="1"/>
+    <col min="3" max="3" width="20.59765625" style="189" customWidth="1"/>
+    <col min="4" max="4" width="14.59765625" customWidth="1"/>
+    <col min="5" max="8" width="12.59765625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="B1" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>250</v>
+      </c>
+      <c r="B2" t="s">
+        <v>249</v>
+      </c>
+      <c r="C2" s="189" t="s">
+        <v>254</v>
+      </c>
+      <c r="D2">
+        <v>24688</v>
+      </c>
+      <c r="E2">
+        <v>-45.7</v>
+      </c>
+      <c r="F2">
+        <v>-44.9</v>
+      </c>
+      <c r="G2">
+        <v>-46.9</v>
+      </c>
+      <c r="H2">
+        <v>-45.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>250</v>
+      </c>
+      <c r="B3" t="s">
+        <v>249</v>
+      </c>
+      <c r="C3" s="189" t="s">
+        <v>255</v>
+      </c>
+      <c r="D3">
+        <v>24585</v>
+      </c>
+      <c r="E3">
+        <v>-45.3</v>
+      </c>
+      <c r="F3">
+        <v>-44.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>250</v>
+      </c>
+      <c r="B4" t="s">
+        <v>249</v>
+      </c>
+      <c r="C4" s="189" t="s">
+        <v>252</v>
+      </c>
+      <c r="D4">
+        <v>24588</v>
+      </c>
+      <c r="E4">
+        <v>-45</v>
+      </c>
+      <c r="F4">
+        <v>-44.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>250</v>
+      </c>
+      <c r="B5" t="s">
+        <v>249</v>
+      </c>
+      <c r="C5" s="189" t="s">
+        <v>251</v>
+      </c>
+      <c r="D5">
+        <v>24691</v>
+      </c>
+      <c r="E5">
+        <v>-44.7</v>
+      </c>
+      <c r="F5">
+        <v>-43.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>250</v>
+      </c>
+      <c r="B6" t="s">
+        <v>249</v>
+      </c>
+      <c r="C6" s="189" t="s">
+        <v>256</v>
+      </c>
+      <c r="D6">
+        <v>24266</v>
+      </c>
+      <c r="E6">
+        <v>-44.7</v>
+      </c>
+      <c r="F6">
+        <v>-43.4</v>
+      </c>
+      <c r="G6">
+        <v>-46.9</v>
+      </c>
+      <c r="H6">
+        <v>-43.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>250</v>
+      </c>
+      <c r="B7" t="s">
+        <v>249</v>
+      </c>
+      <c r="C7" s="189" t="s">
+        <v>260</v>
+      </c>
+      <c r="D7">
+        <v>24684</v>
+      </c>
+      <c r="E7">
+        <v>-44.5</v>
+      </c>
+      <c r="F7">
+        <v>-43.9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>250</v>
+      </c>
+      <c r="B8" t="s">
+        <v>249</v>
+      </c>
+      <c r="C8" s="189" t="s">
+        <v>261</v>
+      </c>
+      <c r="D8">
+        <v>24382</v>
+      </c>
+      <c r="E8">
+        <v>-41.6</v>
+      </c>
+      <c r="F8">
+        <v>-40.299999999999997</v>
+      </c>
+      <c r="G8">
+        <v>-43.8</v>
+      </c>
+      <c r="H8">
+        <v>-42.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
+        <v>250</v>
+      </c>
+      <c r="B9" t="s">
+        <v>249</v>
+      </c>
+      <c r="C9" s="189" t="s">
+        <v>257</v>
+      </c>
+      <c r="D9">
+        <v>24959</v>
+      </c>
+      <c r="E9">
+        <v>-36.9</v>
+      </c>
+      <c r="F9">
+        <v>-37</v>
+      </c>
+      <c r="G9">
+        <v>-40.799999999999997</v>
+      </c>
+      <c r="H9">
+        <v>-38.700000000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
+        <v>250</v>
+      </c>
+      <c r="B10" t="s">
+        <v>249</v>
+      </c>
+      <c r="C10" s="189" t="s">
+        <v>253</v>
+      </c>
+      <c r="D10">
+        <v>31137</v>
+      </c>
+      <c r="E10">
+        <v>-36.6</v>
+      </c>
+      <c r="F10">
+        <v>-36.299999999999997</v>
+      </c>
+      <c r="G10">
+        <v>-37.4</v>
+      </c>
+      <c r="H10">
+        <v>-34.799999999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>250</v>
+      </c>
+      <c r="B11" t="s">
+        <v>249</v>
+      </c>
+      <c r="C11" s="189" t="s">
+        <v>258</v>
+      </c>
+      <c r="D11">
+        <v>24477</v>
+      </c>
+      <c r="E11">
+        <v>-43.7</v>
+      </c>
+      <c r="F11">
+        <v>-43</v>
+      </c>
+      <c r="G11">
+        <v>-44.7</v>
+      </c>
+      <c r="H11">
+        <v>-41.7</v>
+      </c>
+      <c r="I11" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="C15" s="208"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="C16" s="208"/>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.4">
+      <c r="C17" s="208"/>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.4">
+      <c r="C18" s="208"/>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.4">
+      <c r="C19" s="208"/>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.4">
+      <c r="C20" s="208"/>
+    </row>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.4">
+      <c r="C21" s="208"/>
+    </row>
+    <row r="22" spans="3:3" x14ac:dyDescent="0.4">
+      <c r="C22" s="208"/>
+    </row>
+    <row r="23" spans="3:3" x14ac:dyDescent="0.4">
+      <c r="C23" s="208"/>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H18">
+    <sortCondition ref="E2:E18"/>
+    <sortCondition ref="F2:F18"/>
+    <sortCondition ref="G2:G18"/>
+    <sortCondition ref="H2:H18"/>
+  </sortState>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>